<commit_message>
fixed some consistency issue
</commit_message>
<xml_diff>
--- a/src/data/emb_data.xlsx
+++ b/src/data/emb_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andromeda\Desktop\GitHub\LLM-based-QA-chatbot-builder\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\arbit\nlp\chatbot builder\LLM-based-QA-chatbot-builder-main\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A41BF2-8132-449C-8092-A93B9F2E5B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE96FC3-BB77-40F9-9935-A3E3F00B7C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Context</t>
-  </si>
-  <si>
     <t>When was Khulna University of Engineering &amp; Technology (KUET) established?</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>KUET provides a harmonious architectural and natural environment, fostering learning and research excellence.</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>context</t>
   </si>
 </sst>
 </file>
@@ -186,9 +186,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,180 +471,180 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added embedded data generation
</commit_message>
<xml_diff>
--- a/src/data/emb_data.xlsx
+++ b/src/data/emb_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,158 +446,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>label</t>
+          <t>score</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The cat sat on the mat.</t>
+          <t>This is a cat</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The feline rested on the rug.</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>The sun is shining brightly.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>It is raining heavily.</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>She loves to read books.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>She enjoys reading novels.</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>He is a talented musician.</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>He has no musical ability.</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>The car is red.</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>The vehicle is blue.</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>The coffee is hot.</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>The beverage is cold.</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>The dog barked loudly.</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>The canine made a loud noise.</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>The food was delicious.</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>The meal was terrible.</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>He is a skilled programmer.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>He is proficient in coding.</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>The movie was boring.</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>The film was captivating.</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
+          <t>This is a dog</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.7</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>